<commit_message>
Add portfolio allocation simulator and update portfolio analyzer
</commit_message>
<xml_diff>
--- a/Portfolio_Analysis_Sheets.xlsx
+++ b/Portfolio_Analysis_Sheets.xlsx
@@ -613,7 +613,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J53"/>
+  <dimension ref="A1:K54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -631,6 +631,7 @@
     <col width="16" customWidth="1" min="8" max="8"/>
     <col width="16" customWidth="1" min="9" max="9"/>
     <col width="16" customWidth="1" min="10" max="10"/>
+    <col width="16" customWidth="1" min="11" max="11"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -790,6 +791,7 @@
       <c r="H16" s="7" t="n"/>
       <c r="I16" s="7" t="n"/>
       <c r="J16" s="7" t="n"/>
+      <c r="K16" s="7" t="n"/>
     </row>
     <row r="17">
       <c r="A17" s="8" t="inlineStr">
@@ -819,25 +821,30 @@
       </c>
       <c r="F17" s="8" t="inlineStr">
         <is>
+          <t>Simple_Return_%</t>
+        </is>
+      </c>
+      <c r="G17" s="8" t="inlineStr">
+        <is>
           <t>Return_%</t>
         </is>
       </c>
-      <c r="G17" s="8" t="inlineStr">
+      <c r="H17" s="8" t="inlineStr">
         <is>
           <t>Capital</t>
         </is>
       </c>
-      <c r="H17" s="8" t="inlineStr">
+      <c r="I17" s="8" t="inlineStr">
         <is>
           <t>Profit</t>
         </is>
       </c>
-      <c r="I17" s="8" t="inlineStr">
+      <c r="J17" s="8" t="inlineStr">
         <is>
           <t>Max_DD</t>
         </is>
       </c>
-      <c r="J17" s="8" t="inlineStr">
+      <c r="K17" s="8" t="inlineStr">
         <is>
           <t>Years</t>
         </is>
@@ -864,19 +871,23 @@
         <v>19.19</v>
       </c>
       <c r="F18" s="5">
-        <f>ROUND(IF(G18&gt;0, (H18/G18)*100, 0), 2)</f>
-        <v/>
-      </c>
-      <c r="G18" s="5" t="n">
+        <f>ROUND(IF(H18&gt;0, (I18/H18/K18)*100, 0), 2)</f>
+        <v/>
+      </c>
+      <c r="G18" s="5">
+        <f>ROUND(IF(H18&gt;0, (I18/H18)*100, 0), 2)</f>
+        <v/>
+      </c>
+      <c r="H18" s="5" t="n">
         <v>2664</v>
       </c>
-      <c r="H18" s="5" t="n">
+      <c r="I18" s="5" t="n">
         <v>4562.16</v>
       </c>
-      <c r="I18" s="5" t="n">
+      <c r="J18" s="5" t="n">
         <v>1332</v>
       </c>
-      <c r="J18" s="5" t="n">
+      <c r="K18" s="5" t="n">
         <v>5.7</v>
       </c>
     </row>
@@ -901,19 +912,23 @@
         <v>21.7</v>
       </c>
       <c r="F19" s="5">
-        <f>ROUND(IF(G19&gt;0, (H19/G19)*100, 0), 2)</f>
-        <v/>
-      </c>
-      <c r="G19" s="5" t="n">
+        <f>ROUND(IF(H19&gt;0, (I19/H19/K19)*100, 0), 2)</f>
+        <v/>
+      </c>
+      <c r="G19" s="5">
+        <f>ROUND(IF(H19&gt;0, (I19/H19)*100, 0), 2)</f>
+        <v/>
+      </c>
+      <c r="H19" s="5" t="n">
         <v>6832</v>
       </c>
-      <c r="H19" s="5" t="n">
+      <c r="I19" s="5" t="n">
         <v>9441.959999999999</v>
       </c>
-      <c r="I19" s="5" t="n">
+      <c r="J19" s="5" t="n">
         <v>3416</v>
       </c>
-      <c r="J19" s="5" t="n">
+      <c r="K19" s="5" t="n">
         <v>4.89</v>
       </c>
     </row>
@@ -938,19 +953,23 @@
         <v>22.04</v>
       </c>
       <c r="F20" s="5">
-        <f>ROUND(IF(G20&gt;0, (H20/G20)*100, 0), 2)</f>
-        <v/>
-      </c>
-      <c r="G20" s="5" t="n">
+        <f>ROUND(IF(H20&gt;0, (I20/H20/K20)*100, 0), 2)</f>
+        <v/>
+      </c>
+      <c r="G20" s="5">
+        <f>ROUND(IF(H20&gt;0, (I20/H20)*100, 0), 2)</f>
+        <v/>
+      </c>
+      <c r="H20" s="5" t="n">
         <v>5312.2</v>
       </c>
-      <c r="H20" s="5" t="n">
+      <c r="I20" s="5" t="n">
         <v>6590.47</v>
       </c>
-      <c r="I20" s="5" t="n">
+      <c r="J20" s="5" t="n">
         <v>2656.1</v>
       </c>
-      <c r="J20" s="5" t="n">
+      <c r="K20" s="5" t="n">
         <v>5.22</v>
       </c>
     </row>
@@ -975,19 +994,23 @@
         <v>13.34</v>
       </c>
       <c r="F21" s="5">
-        <f>ROUND(IF(G21&gt;0, (H21/G21)*100, 0), 2)</f>
-        <v/>
-      </c>
-      <c r="G21" s="5" t="n">
+        <f>ROUND(IF(H21&gt;0, (I21/H21/K21)*100, 0), 2)</f>
+        <v/>
+      </c>
+      <c r="G21" s="5">
+        <f>ROUND(IF(H21&gt;0, (I21/H21)*100, 0), 2)</f>
+        <v/>
+      </c>
+      <c r="H21" s="5" t="n">
         <v>206.04</v>
       </c>
-      <c r="H21" s="5" t="n">
+      <c r="I21" s="5" t="n">
         <v>164.25</v>
       </c>
-      <c r="I21" s="5" t="n">
+      <c r="J21" s="5" t="n">
         <v>103.02</v>
       </c>
-      <c r="J21" s="5" t="n">
+      <c r="K21" s="5" t="n">
         <v>5.91</v>
       </c>
     </row>
@@ -1012,19 +1035,23 @@
         <v>11.14</v>
       </c>
       <c r="F22" s="5">
-        <f>ROUND(IF(G22&gt;0, (H22/G22)*100, 0), 2)</f>
-        <v/>
-      </c>
-      <c r="G22" s="5" t="n">
+        <f>ROUND(IF(H22&gt;0, (I22/H22/K22)*100, 0), 2)</f>
+        <v/>
+      </c>
+      <c r="G22" s="5">
+        <f>ROUND(IF(H22&gt;0, (I22/H22)*100, 0), 2)</f>
+        <v/>
+      </c>
+      <c r="H22" s="5" t="n">
         <v>15494.74</v>
       </c>
-      <c r="H22" s="5" t="n">
+      <c r="I22" s="5" t="n">
         <v>5461.52</v>
       </c>
-      <c r="I22" s="5" t="n">
+      <c r="J22" s="5" t="n">
         <v>7747.37</v>
       </c>
-      <c r="J22" s="5" t="n">
+      <c r="K22" s="5" t="n">
         <v>5.53</v>
       </c>
     </row>
@@ -1049,19 +1076,23 @@
         <v>14.34</v>
       </c>
       <c r="F23" s="5">
-        <f>ROUND(IF(G23&gt;0, (H23/G23)*100, 0), 2)</f>
-        <v/>
-      </c>
-      <c r="G23" s="5" t="n">
+        <f>ROUND(IF(H23&gt;0, (I23/H23/K23)*100, 0), 2)</f>
+        <v/>
+      </c>
+      <c r="G23" s="5">
+        <f>ROUND(IF(H23&gt;0, (I23/H23)*100, 0), 2)</f>
+        <v/>
+      </c>
+      <c r="H23" s="5" t="n">
         <v>20142</v>
       </c>
-      <c r="H23" s="5" t="n">
+      <c r="I23" s="5" t="n">
         <v>27715.57</v>
       </c>
-      <c r="I23" s="5" t="n">
+      <c r="J23" s="5" t="n">
         <v>10071</v>
       </c>
-      <c r="J23" s="5" t="n">
+      <c r="K23" s="5" t="n">
         <v>5.73</v>
       </c>
     </row>
@@ -1086,19 +1117,23 @@
         <v>15.01</v>
       </c>
       <c r="F24" s="5">
-        <f>ROUND(IF(G24&gt;0, (H24/G24)*100, 0), 2)</f>
-        <v/>
-      </c>
-      <c r="G24" s="5" t="n">
+        <f>ROUND(IF(H24&gt;0, (I24/H24/K24)*100, 0), 2)</f>
+        <v/>
+      </c>
+      <c r="G24" s="5">
+        <f>ROUND(IF(H24&gt;0, (I24/H24)*100, 0), 2)</f>
+        <v/>
+      </c>
+      <c r="H24" s="5" t="n">
         <v>25358</v>
       </c>
-      <c r="H24" s="5" t="n">
+      <c r="I24" s="5" t="n">
         <v>36428.76</v>
       </c>
-      <c r="I24" s="5" t="n">
+      <c r="J24" s="5" t="n">
         <v>12679</v>
       </c>
-      <c r="J24" s="5" t="n">
+      <c r="K24" s="5" t="n">
         <v>5.68</v>
       </c>
     </row>
@@ -1123,19 +1158,23 @@
         <v>16.25</v>
       </c>
       <c r="F25" s="5">
-        <f>ROUND(IF(G25&gt;0, (H25/G25)*100, 0), 2)</f>
-        <v/>
-      </c>
-      <c r="G25" s="5" t="n">
+        <f>ROUND(IF(H25&gt;0, (I25/H25/K25)*100, 0), 2)</f>
+        <v/>
+      </c>
+      <c r="G25" s="5">
+        <f>ROUND(IF(H25&gt;0, (I25/H25)*100, 0), 2)</f>
+        <v/>
+      </c>
+      <c r="H25" s="5" t="n">
         <v>820</v>
       </c>
-      <c r="H25" s="5" t="n">
+      <c r="I25" s="5" t="n">
         <v>1200.98</v>
       </c>
-      <c r="I25" s="5" t="n">
+      <c r="J25" s="5" t="n">
         <v>410</v>
       </c>
-      <c r="J25" s="5" t="n">
+      <c r="K25" s="5" t="n">
         <v>5.99</v>
       </c>
     </row>
@@ -1153,10 +1192,7 @@
       <c r="D26" s="9" t="n"/>
       <c r="E26" s="9" t="n"/>
       <c r="F26" s="9" t="n"/>
-      <c r="G26" s="9">
-        <f>ROUND(SUM(G18:G25), 2)</f>
-        <v/>
-      </c>
+      <c r="G26" s="9" t="n"/>
       <c r="H26" s="9">
         <f>ROUND(SUM(H18:H25), 2)</f>
         <v/>
@@ -1165,7 +1201,11 @@
         <f>ROUND(SUM(I18:I25), 2)</f>
         <v/>
       </c>
-      <c r="J26" s="9" t="n"/>
+      <c r="J26" s="9">
+        <f>ROUND(SUM(J18:J25), 2)</f>
+        <v/>
+      </c>
+      <c r="K26" s="9" t="n"/>
     </row>
     <row r="29">
       <c r="A29" s="10" t="inlineStr">
@@ -1234,11 +1274,11 @@
         <v/>
       </c>
       <c r="C31" s="5">
-        <f>ROUND((B31/100)*$G$26, 2)</f>
+        <f>ROUND((B31/100)*$H$26, 2)</f>
         <v/>
       </c>
       <c r="D31" s="5">
-        <f>ROUND(G18, 2)</f>
+        <f>ROUND(H18, 2)</f>
         <v/>
       </c>
       <c r="E31" s="5">
@@ -1269,11 +1309,11 @@
         <v/>
       </c>
       <c r="C32" s="5">
-        <f>ROUND((B32/100)*$G$26, 2)</f>
+        <f>ROUND((B32/100)*$H$26, 2)</f>
         <v/>
       </c>
       <c r="D32" s="5">
-        <f>ROUND(G19, 2)</f>
+        <f>ROUND(H19, 2)</f>
         <v/>
       </c>
       <c r="E32" s="5">
@@ -1304,11 +1344,11 @@
         <v/>
       </c>
       <c r="C33" s="5">
-        <f>ROUND((B33/100)*$G$26, 2)</f>
+        <f>ROUND((B33/100)*$H$26, 2)</f>
         <v/>
       </c>
       <c r="D33" s="5">
-        <f>ROUND(G20, 2)</f>
+        <f>ROUND(H20, 2)</f>
         <v/>
       </c>
       <c r="E33" s="5">
@@ -1339,11 +1379,11 @@
         <v/>
       </c>
       <c r="C34" s="5">
-        <f>ROUND((B34/100)*$G$26, 2)</f>
+        <f>ROUND((B34/100)*$H$26, 2)</f>
         <v/>
       </c>
       <c r="D34" s="5">
-        <f>ROUND(G21, 2)</f>
+        <f>ROUND(H21, 2)</f>
         <v/>
       </c>
       <c r="E34" s="5">
@@ -1374,11 +1414,11 @@
         <v/>
       </c>
       <c r="C35" s="5">
-        <f>ROUND((B35/100)*$G$26, 2)</f>
+        <f>ROUND((B35/100)*$H$26, 2)</f>
         <v/>
       </c>
       <c r="D35" s="5">
-        <f>ROUND(G22, 2)</f>
+        <f>ROUND(H22, 2)</f>
         <v/>
       </c>
       <c r="E35" s="5">
@@ -1409,11 +1449,11 @@
         <v/>
       </c>
       <c r="C36" s="5">
-        <f>ROUND((B36/100)*$G$26, 2)</f>
+        <f>ROUND((B36/100)*$H$26, 2)</f>
         <v/>
       </c>
       <c r="D36" s="5">
-        <f>ROUND(G23, 2)</f>
+        <f>ROUND(H23, 2)</f>
         <v/>
       </c>
       <c r="E36" s="5">
@@ -1444,11 +1484,11 @@
         <v/>
       </c>
       <c r="C37" s="5">
-        <f>ROUND((B37/100)*$G$26, 2)</f>
+        <f>ROUND((B37/100)*$H$26, 2)</f>
         <v/>
       </c>
       <c r="D37" s="5">
-        <f>ROUND(G24, 2)</f>
+        <f>ROUND(H24, 2)</f>
         <v/>
       </c>
       <c r="E37" s="5">
@@ -1479,11 +1519,11 @@
         <v/>
       </c>
       <c r="C38" s="5">
-        <f>ROUND((B38/100)*$G$26, 2)</f>
+        <f>ROUND((B38/100)*$H$26, 2)</f>
         <v/>
       </c>
       <c r="D38" s="5">
-        <f>ROUND(G25, 2)</f>
+        <f>ROUND(H25, 2)</f>
         <v/>
       </c>
       <c r="E38" s="5">
@@ -1557,7 +1597,7 @@
         </is>
       </c>
       <c r="B44" s="5">
-        <f>ROUND(G26, 2)</f>
+        <f>ROUND(H26, 2)</f>
         <v/>
       </c>
       <c r="C44" s="5" t="inlineStr">
@@ -1573,7 +1613,7 @@
         </is>
       </c>
       <c r="B45" s="5">
-        <f>ROUND(I26, 2)</f>
+        <f>ROUND(J26, 2)</f>
         <v/>
       </c>
       <c r="C45" s="5" t="inlineStr">
@@ -1617,51 +1657,67 @@
     <row r="48">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>Expected Total Profit</t>
+          <t>Portfolio Simple Return %</t>
         </is>
       </c>
       <c r="B48" s="5">
-        <f>ROUND(H26, 2)</f>
+        <f>ROUND(SUMPRODUCT(B31:B38/100, F18:F25), 2)</f>
         <v/>
       </c>
       <c r="C48" s="5" t="inlineStr">
         <is>
-          <t>$</t>
+          <t>%</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="3" t="inlineStr">
         <is>
+          <t>Expected Total Profit</t>
+        </is>
+      </c>
+      <c r="B49" s="5">
+        <f>ROUND(I26, 2)</f>
+        <v/>
+      </c>
+      <c r="C49" s="5" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="3" t="inlineStr">
+        <is>
           <t>Overall Return on Capital</t>
         </is>
       </c>
-      <c r="B49" s="5">
-        <f>ROUND(IF(G26&gt;0, (H26/G26)*100, 0), 2)</f>
-        <v/>
-      </c>
-      <c r="C49" s="5" t="inlineStr">
+      <c r="B50" s="5">
+        <f>ROUND(IF(H26&gt;0, (I26/H26)*100, 0), 2)</f>
+        <v/>
+      </c>
+      <c r="C50" s="5" t="inlineStr">
         <is>
           <t>%</t>
         </is>
       </c>
     </row>
-    <row r="51">
-      <c r="A51" s="14" t="inlineStr">
+    <row r="52">
+      <c r="A52" s="14" t="inlineStr">
         <is>
           <t>SHARPE RATIO FORMULA:</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" s="15" t="inlineStr">
-        <is>
-          <t>Portfolio Sharpe = Σ(Weight_i × Sharpe_i)</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="15" t="inlineStr">
+        <is>
+          <t>Portfolio Sharpe = Σ(Weight_i × Sharpe_i)</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="15" t="inlineStr">
         <is>
           <t>Where Sharpe_i = (Mean Profit / Std Dev) × √(Trades per Year)</t>
         </is>
@@ -1672,8 +1728,8 @@
     <mergeCell ref="A42:C42"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A29:H29"/>
+    <mergeCell ref="A16:K16"/>
     <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A16:J16"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio analysis tools and add yearly returns analyzer
</commit_message>
<xml_diff>
--- a/Portfolio_Analysis_Sheets.xlsx
+++ b/Portfolio_Analysis_Sheets.xlsx
@@ -675,7 +675,7 @@
     <row r="6">
       <c r="A6" s="5" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • 7th_Strategy:</t>
+          <t xml:space="preserve">  • Golden Stallion:</t>
         </is>
       </c>
       <c r="B6" s="6" t="inlineStr">
@@ -688,7 +688,7 @@
     <row r="7">
       <c r="A7" s="5" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • Falcon:</t>
+          <t xml:space="preserve">  • Silver Falcon:</t>
         </is>
       </c>
       <c r="B7" s="6" t="inlineStr">
@@ -701,7 +701,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • Gold_Dip:</t>
+          <t xml:space="preserve">  • Iron Bear:</t>
         </is>
       </c>
       <c r="B8" s="6" t="inlineStr">
@@ -714,7 +714,7 @@
     <row r="9">
       <c r="A9" s="5" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • RSI_Correlation:</t>
+          <t xml:space="preserve">  • Night Wolf:</t>
         </is>
       </c>
       <c r="B9" s="6" t="inlineStr">
@@ -727,7 +727,7 @@
     <row r="10">
       <c r="A10" s="5" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • RSI_6_Trades:</t>
+          <t xml:space="preserve">  • Red Kraken:</t>
         </is>
       </c>
       <c r="B10" s="6" t="inlineStr">
@@ -740,7 +740,7 @@
     <row r="11">
       <c r="A11" s="5" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • AURUM:</t>
+          <t xml:space="preserve">  • Black Dragon:</t>
         </is>
       </c>
       <c r="B11" s="6" t="inlineStr">
@@ -753,7 +753,7 @@
     <row r="12">
       <c r="A12" s="5" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • PairTradingEA:</t>
+          <t xml:space="preserve">  • Twin Fox:</t>
         </is>
       </c>
       <c r="B12" s="6" t="inlineStr">
@@ -766,7 +766,7 @@
     <row r="13">
       <c r="A13" s="5" t="inlineStr">
         <is>
-          <t xml:space="preserve">  • Reversal_Strategy:</t>
+          <t xml:space="preserve">  • Shadow Owl:</t>
         </is>
       </c>
       <c r="B13" s="6" t="inlineStr">
@@ -853,7 +853,7 @@
     <row r="18">
       <c r="A18" s="5" t="inlineStr">
         <is>
-          <t>7th_Strategy</t>
+          <t>Golden Stallion</t>
         </is>
       </c>
       <c r="B18" s="5" t="inlineStr">
@@ -894,7 +894,7 @@
     <row r="19">
       <c r="A19" s="5" t="inlineStr">
         <is>
-          <t>Falcon</t>
+          <t>Silver Falcon</t>
         </is>
       </c>
       <c r="B19" s="5" t="inlineStr">
@@ -935,7 +935,7 @@
     <row r="20">
       <c r="A20" s="5" t="inlineStr">
         <is>
-          <t>Gold_Dip</t>
+          <t>Iron Bear</t>
         </is>
       </c>
       <c r="B20" s="5" t="inlineStr">
@@ -976,7 +976,7 @@
     <row r="21">
       <c r="A21" s="5" t="inlineStr">
         <is>
-          <t>RSI_Correlation</t>
+          <t>Night Wolf</t>
         </is>
       </c>
       <c r="B21" s="5" t="inlineStr">
@@ -1017,7 +1017,7 @@
     <row r="22">
       <c r="A22" s="5" t="inlineStr">
         <is>
-          <t>RSI_6_Trades</t>
+          <t>Red Kraken</t>
         </is>
       </c>
       <c r="B22" s="5" t="inlineStr">
@@ -1058,7 +1058,7 @@
     <row r="23">
       <c r="A23" s="5" t="inlineStr">
         <is>
-          <t>AURUM</t>
+          <t>Black Dragon</t>
         </is>
       </c>
       <c r="B23" s="5" t="inlineStr">
@@ -1099,7 +1099,7 @@
     <row r="24">
       <c r="A24" s="5" t="inlineStr">
         <is>
-          <t>PairTradingEA</t>
+          <t>Twin Fox</t>
         </is>
       </c>
       <c r="B24" s="5" t="inlineStr">
@@ -1140,7 +1140,7 @@
     <row r="25">
       <c r="A25" s="5" t="inlineStr">
         <is>
-          <t>Reversal_Strategy</t>
+          <t>Shadow Owl</t>
         </is>
       </c>
       <c r="B25" s="5" t="inlineStr">
@@ -1266,7 +1266,7 @@
     <row r="31">
       <c r="A31" s="5" t="inlineStr">
         <is>
-          <t>7th_Strategy</t>
+          <t>Golden Stallion</t>
         </is>
       </c>
       <c r="B31" s="5">
@@ -1301,7 +1301,7 @@
     <row r="32">
       <c r="A32" s="5" t="inlineStr">
         <is>
-          <t>Falcon</t>
+          <t>Silver Falcon</t>
         </is>
       </c>
       <c r="B32" s="5">
@@ -1336,7 +1336,7 @@
     <row r="33">
       <c r="A33" s="5" t="inlineStr">
         <is>
-          <t>Gold_Dip</t>
+          <t>Iron Bear</t>
         </is>
       </c>
       <c r="B33" s="5">
@@ -1371,7 +1371,7 @@
     <row r="34">
       <c r="A34" s="5" t="inlineStr">
         <is>
-          <t>RSI_Correlation</t>
+          <t>Night Wolf</t>
         </is>
       </c>
       <c r="B34" s="5">
@@ -1406,7 +1406,7 @@
     <row r="35">
       <c r="A35" s="5" t="inlineStr">
         <is>
-          <t>RSI_6_Trades</t>
+          <t>Red Kraken</t>
         </is>
       </c>
       <c r="B35" s="5">
@@ -1441,7 +1441,7 @@
     <row r="36">
       <c r="A36" s="5" t="inlineStr">
         <is>
-          <t>AURUM</t>
+          <t>Black Dragon</t>
         </is>
       </c>
       <c r="B36" s="5">
@@ -1476,7 +1476,7 @@
     <row r="37">
       <c r="A37" s="5" t="inlineStr">
         <is>
-          <t>PairTradingEA</t>
+          <t>Twin Fox</t>
         </is>
       </c>
       <c r="B37" s="5">
@@ -1511,7 +1511,7 @@
     <row r="38">
       <c r="A38" s="5" t="inlineStr">
         <is>
-          <t>Reversal_Strategy</t>
+          <t>Shadow Owl</t>
         </is>
       </c>
       <c r="B38" s="5">
@@ -1786,7 +1786,7 @@
     <row r="4">
       <c r="A4" s="7" t="inlineStr">
         <is>
-          <t>Strategy: 7th_Strategy</t>
+          <t>Strategy: Golden Stallion</t>
         </is>
       </c>
       <c r="B4" s="7" t="n"/>
@@ -2103,7 +2103,7 @@
     <row r="11">
       <c r="A11" s="10" t="inlineStr">
         <is>
-          <t>Strategy: Falcon</t>
+          <t>Strategy: Silver Falcon</t>
         </is>
       </c>
       <c r="B11" s="10" t="n"/>
@@ -2420,7 +2420,7 @@
     <row r="18">
       <c r="A18" s="11" t="inlineStr">
         <is>
-          <t>Strategy: Gold_Dip</t>
+          <t>Strategy: Iron Bear</t>
         </is>
       </c>
       <c r="B18" s="11" t="n"/>
@@ -3151,7 +3151,7 @@
     <row r="31">
       <c r="A31" s="18" t="inlineStr">
         <is>
-          <t>Strategy: RSI_Correlation</t>
+          <t>Strategy: Night Wolf</t>
         </is>
       </c>
       <c r="B31" s="18" t="n"/>
@@ -3744,7 +3744,7 @@
     <row r="42">
       <c r="A42" s="19" t="inlineStr">
         <is>
-          <t>Strategy: RSI_6_Trades</t>
+          <t>Strategy: Red Kraken</t>
         </is>
       </c>
       <c r="B42" s="19" t="n"/>
@@ -4958,7 +4958,7 @@
     <row r="62">
       <c r="A62" s="20" t="inlineStr">
         <is>
-          <t>Strategy: AURUM</t>
+          <t>Strategy: Black Dragon</t>
         </is>
       </c>
       <c r="B62" s="20" t="n"/>
@@ -5275,7 +5275,7 @@
     <row r="69">
       <c r="A69" s="21" t="inlineStr">
         <is>
-          <t>Strategy: PairTradingEA</t>
+          <t>Strategy: Twin Fox</t>
         </is>
       </c>
       <c r="B69" s="21" t="n"/>
@@ -5799,7 +5799,7 @@
     <row r="79">
       <c r="A79" s="22" t="inlineStr">
         <is>
-          <t>Strategy: Reversal_Strategy</t>
+          <t>Strategy: Shadow Owl</t>
         </is>
       </c>
       <c r="B79" s="22" t="n"/>
@@ -6099,7 +6099,7 @@
     <row r="3">
       <c r="A3" s="7" t="inlineStr">
         <is>
-          <t>STRATEGY: 7th_Strategy (2 pairs)</t>
+          <t>STRATEGY: Golden Stallion (2 pairs)</t>
         </is>
       </c>
       <c r="B3" s="7" t="n"/>
@@ -6312,7 +6312,7 @@
     <row r="10">
       <c r="A10" s="10" t="inlineStr">
         <is>
-          <t>STRATEGY: Falcon (2 pairs)</t>
+          <t>STRATEGY: Silver Falcon (2 pairs)</t>
         </is>
       </c>
       <c r="B10" s="10" t="n"/>
@@ -6525,7 +6525,7 @@
     <row r="17">
       <c r="A17" s="11" t="inlineStr">
         <is>
-          <t>STRATEGY: Gold_Dip (8 pairs)</t>
+          <t>STRATEGY: Iron Bear (8 pairs)</t>
         </is>
       </c>
       <c r="B17" s="11" t="n"/>
@@ -7002,7 +7002,7 @@
     <row r="30">
       <c r="A30" s="18" t="inlineStr">
         <is>
-          <t>STRATEGY: RSI_Correlation (6 pairs)</t>
+          <t>STRATEGY: Night Wolf (6 pairs)</t>
         </is>
       </c>
       <c r="B30" s="18" t="n"/>
@@ -7391,7 +7391,7 @@
     <row r="41">
       <c r="A41" s="19" t="inlineStr">
         <is>
-          <t>STRATEGY: RSI_6_Trades (15 pairs)</t>
+          <t>STRATEGY: Red Kraken (15 pairs)</t>
         </is>
       </c>
       <c r="B41" s="19" t="n"/>
@@ -8176,7 +8176,7 @@
     <row r="61">
       <c r="A61" s="20" t="inlineStr">
         <is>
-          <t>STRATEGY: AURUM (2 pairs)</t>
+          <t>STRATEGY: Black Dragon (2 pairs)</t>
         </is>
       </c>
       <c r="B61" s="20" t="n"/>
@@ -8389,7 +8389,7 @@
     <row r="68">
       <c r="A68" s="21" t="inlineStr">
         <is>
-          <t>STRATEGY: PairTradingEA (5 pairs)</t>
+          <t>STRATEGY: Twin Fox (5 pairs)</t>
         </is>
       </c>
       <c r="B68" s="21" t="n"/>
@@ -8734,7 +8734,7 @@
     <row r="78">
       <c r="A78" s="22" t="inlineStr">
         <is>
-          <t>STRATEGY: Reversal_Strategy (1 pairs)</t>
+          <t>STRATEGY: Shadow Owl (1 pairs)</t>
         </is>
       </c>
       <c r="B78" s="22" t="n"/>
@@ -9034,7 +9034,7 @@
     <row r="5">
       <c r="A5" s="5" t="inlineStr">
         <is>
-          <t>7th_Strategy</t>
+          <t>Golden Stallion</t>
         </is>
       </c>
       <c r="B5" s="5" t="n">
@@ -9077,7 +9077,7 @@
     <row r="6">
       <c r="A6" s="5" t="inlineStr">
         <is>
-          <t>Falcon</t>
+          <t>Silver Falcon</t>
         </is>
       </c>
       <c r="B6" s="5" t="n">
@@ -9120,7 +9120,7 @@
     <row r="7">
       <c r="A7" s="5" t="inlineStr">
         <is>
-          <t>Gold_Dip</t>
+          <t>Iron Bear</t>
         </is>
       </c>
       <c r="B7" s="5" t="n">
@@ -9163,7 +9163,7 @@
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
-          <t>RSI_Correlation</t>
+          <t>Night Wolf</t>
         </is>
       </c>
       <c r="B8" s="5" t="n">
@@ -9206,7 +9206,7 @@
     <row r="9">
       <c r="A9" s="5" t="inlineStr">
         <is>
-          <t>RSI_6_Trades</t>
+          <t>Red Kraken</t>
         </is>
       </c>
       <c r="B9" s="5" t="n">
@@ -9249,7 +9249,7 @@
     <row r="10">
       <c r="A10" s="5" t="inlineStr">
         <is>
-          <t>AURUM</t>
+          <t>Black Dragon</t>
         </is>
       </c>
       <c r="B10" s="5" t="n">
@@ -9292,7 +9292,7 @@
     <row r="11">
       <c r="A11" s="5" t="inlineStr">
         <is>
-          <t>PairTradingEA</t>
+          <t>Twin Fox</t>
         </is>
       </c>
       <c r="B11" s="5" t="n">
@@ -9335,7 +9335,7 @@
     <row r="12">
       <c r="A12" s="5" t="inlineStr">
         <is>
-          <t>Reversal_Strategy</t>
+          <t>Shadow Owl</t>
         </is>
       </c>
       <c r="B12" s="5" t="n">

</xml_diff>